<commit_message>
Tested RequireNonZero in 3 different optimizer scenarios
</commit_message>
<xml_diff>
--- a/docs/data/examples/Gas optimisations.xlsx
+++ b/docs/data/examples/Gas optimisations.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\examples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FA334D-5C1A-4856-9266-570239945FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RequireNonZero" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +24,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+  <si>
+    <t>Optimizer disabled</t>
+  </si>
+  <si>
+    <t>requireLargerThanZero</t>
+  </si>
+  <si>
+    <t>requireNotEqualsZero</t>
+  </si>
+  <si>
+    <t>gas consumed</t>
+  </si>
+  <si>
+    <t>Optimizer enabled - 200 runs</t>
+  </si>
+  <si>
+    <t>Optimizer enabled - 1000 runs</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +57,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,15 +107,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +440,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C3:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" style="1"/>
+    <col min="3" max="3" width="35.7109375" style="1" customWidth="1"/>
+    <col min="4" max="6" width="20.7109375" style="1"/>
+    <col min="7" max="7" width="35.7109375" style="1" customWidth="1"/>
+    <col min="8" max="10" width="20.7109375" style="1"/>
+    <col min="11" max="11" width="35.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="20.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>716</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>351</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>694</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>324</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="3:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>